<commit_message>
Updated Code as instructed in GitHub Comments
</commit_message>
<xml_diff>
--- a/ExcelExamples/BesaJSECPIBond.xlsx
+++ b/ExcelExamples/BesaJSECPIBond.xlsx
@@ -8,18 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\QSA008\ExcelExamples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{458770F0-6FC6-4C2B-875C-1E75309009E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FBA0ABD-FE9E-4375-9316-C5DF65559F33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{22AAC177-9997-449C-8BA1-AEA9B7E68A8A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{22AAC177-9997-449C-8BA1-AEA9B7E68A8A}"/>
   </bookViews>
   <sheets>
     <sheet name="createBesaJSEBond" sheetId="2" r:id="rId1"/>
     <sheet name="Bond Parameters" sheetId="4" r:id="rId2"/>
-    <sheet name="createBesaJseCPIBond" sheetId="5" r:id="rId3"/>
-    <sheet name="Pricing" sheetId="6" r:id="rId4"/>
+    <sheet name="createBesaJseCPIBond + Pricing" sheetId="5" r:id="rId3"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId5"/>
+    <externalReference r:id="rId4"/>
   </externalReferences>
   <definedNames>
     <definedName name="ZARHols">'[1]ZAR Public Holidays'!$D$9:$D$261</definedName>
@@ -65,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t>name</t>
   </si>
@@ -116,6 +115,27 @@
   </si>
   <si>
     <t>QSA.BesaJSEBondResults</t>
+  </si>
+  <si>
+    <t>settlementDate</t>
+  </si>
+  <si>
+    <t>issueDate</t>
+  </si>
+  <si>
+    <t>cpiIssue</t>
+  </si>
+  <si>
+    <t>cpiSettlement</t>
+  </si>
+  <si>
+    <t>QSA.CreateBesaJSECPIBond</t>
+  </si>
+  <si>
+    <t>underlyingBond</t>
+  </si>
+  <si>
+    <t>besaJseCPIBond</t>
   </si>
 </sst>
 </file>
@@ -151,7 +171,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -182,6 +202,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -196,7 +222,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -208,6 +234,7 @@
     <xf numFmtId="14" fontId="0" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1819,7 +1846,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5A0B17B-E05F-4E28-B413-8FFFEB4FFDED}">
   <dimension ref="B2:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -1850,7 +1877,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="5">
-        <v>47514</v>
+        <v>45688</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
@@ -1866,7 +1893,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="6">
-        <v>0.08</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
@@ -1906,7 +1933,7 @@
         <v>12</v>
       </c>
       <c r="C11" s="4">
-        <v>10</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="2:3" ht="21" x14ac:dyDescent="0.35">
@@ -1917,7 +1944,7 @@
     <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="str" cm="1">
         <f t="array" ref="B14">_xll.QSA.CreateBesaJSEBond(C2,C4,C5,C6,C7,C8,C9,C10,C11,C3)</f>
-        <v>besaJseBond.22:52:22-1</v>
+        <v>besaJseBond.16:08:38-1</v>
       </c>
     </row>
   </sheetData>
@@ -1931,7 +1958,7 @@
   <dimension ref="B2:C11"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1948,7 +1975,7 @@
       </c>
       <c r="C2" s="4" t="str">
         <f>createBesaJSEBond!B14</f>
-        <v>besaJseBond.22:52:22-1</v>
+        <v>besaJseBond.16:08:38-1</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
@@ -1956,7 +1983,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="8">
-        <v>42432</v>
+        <v>44188</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
@@ -1964,7 +1991,7 @@
         <v>13</v>
       </c>
       <c r="C4" s="7">
-        <v>9.7000000000000003E-2</v>
+        <v>2.7E-2</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="21" x14ac:dyDescent="0.35">
@@ -1978,7 +2005,7 @@
         <v>roundedAip</v>
       </c>
       <c r="C7" s="9" t="str">
-        <v>87.85608</v>
+        <v>98,08354</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
@@ -1986,7 +2013,7 @@
         <v>unroundedAip</v>
       </c>
       <c r="C8" s="9" t="str">
-        <v>87.8560780776516</v>
+        <v>98,0835441951121</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">
@@ -1994,7 +2021,7 @@
         <v>roundedClean</v>
       </c>
       <c r="C9" s="9" t="str">
-        <v>87.15471</v>
+        <v>97,28902</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
@@ -2002,7 +2029,7 @@
         <v>unroundedClean</v>
       </c>
       <c r="C10" s="9" t="str">
-        <v>87.1547082146379</v>
+        <v>97,2890236471669</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.25">
@@ -2010,7 +2037,7 @@
         <v>unroundedAccrued</v>
       </c>
       <c r="C11" s="9" t="str">
-        <v>0.701369863013699</v>
+        <v>0,794520547945205</v>
       </c>
     </row>
   </sheetData>
@@ -2021,24 +2048,95 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46339BEA-6997-4709-B7E5-4972D36F0DD4}">
-  <dimension ref="A1"/>
+  <dimension ref="B2:J11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7404E2F0-9486-4021-BC90-39C95406355B}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="36.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="4" t="str">
+        <f>createBesaJSEBond!B14</f>
+        <v>besaJseBond.16:08:38-1</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="4">
+        <v>77.599999999999994</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" s="4">
+        <v>116.6</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="5">
+        <f>'Bond Parameters'!C3</f>
+        <v>44188</v>
+      </c>
+      <c r="F3" s="4">
+        <v>77.900000000000006</v>
+      </c>
+      <c r="J3" s="4">
+        <v>116.8</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="5">
+        <v>41094</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" ht="21" x14ac:dyDescent="0.35">
+      <c r="B7" s="10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="str" cm="1">
+        <f t="array" ref="B8">_xll.QSA.CreateBesaJSECPIBond(C5,C2,F2:F3,J2:J3,C4,C3)</f>
+        <v>besaJseCPIBond.16:08:38-2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" ht="21" x14ac:dyDescent="0.35">
+      <c r="B10" s="10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="11" cm="1">
+        <f t="array" ref="B11">_xll.QSA.BesaJSECPIBondPrice(B8,J2:J3,F2:F3,'Bond Parameters'!C4)</f>
+        <v>147.50232</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>